<commit_message>
Update Spacecraft Operational Modes.xlsx
</commit_message>
<xml_diff>
--- a/Spacecraft Operational Modes.xlsx
+++ b/Spacecraft Operational Modes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28816"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28824"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://curtin.sharepoint.com/sites/SpaceSystemsDesign2/Shared Documents/General/2. Assessments/Assessment Instructions/Assessment One - Space Mission Design Project/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FAC5989-FDD0-4794-92CC-7208EDFACDD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{35C706EA-0F03-439B-8C28-C07111568A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22800" yWindow="6270" windowWidth="32895" windowHeight="17895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -95,7 +95,7 @@
     <t>Actuator to apply pressure to heating chamber</t>
   </si>
   <si>
-    <t>Sintering compression</t>
+    <t>Compression</t>
   </si>
   <si>
     <t>Testing compression</t>
@@ -797,7 +797,7 @@
         <v>15</v>
       </c>
       <c r="H5" s="12">
-        <v>100</v>
+        <v>750</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>16</v>
@@ -826,16 +826,16 @@
         <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="12">
+        <v>140</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="12">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="H6" s="12">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>14</v>
@@ -847,7 +847,7 @@
         <v>20</v>
       </c>
       <c r="L6" s="12">
-        <v>100</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1047,12 +1047,12 @@
       <c r="E12" s="1"/>
       <c r="F12" s="12">
         <f>SUM(F4:F11)</f>
-        <v>360</v>
+        <v>500</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="12">
         <f>SUM(H4:H11)</f>
-        <v>205</v>
+        <v>805</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="12">
@@ -1062,7 +1062,7 @@
       <c r="K12" s="1"/>
       <c r="L12" s="12">
         <f>SUM(L4:L11)</f>
-        <v>195</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -1080,17 +1080,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a6b3153b-6211-49e8-b9df-4ed7471cd786">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b68631fe-1afa-4047-a259-e724fa491ab9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1099,7 +1088,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FB2862965B20C44C943B8CAA8223E757" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4be44708f884c9269ac4b126b93f22dd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a6b3153b-6211-49e8-b9df-4ed7471cd786" xmlns:ns3="b68631fe-1afa-4047-a259-e724fa491ab9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="33fa2d1334b7584d123de97903261f7e" ns2:_="" ns3:_="">
     <xsd:import namespace="a6b3153b-6211-49e8-b9df-4ed7471cd786"/>
@@ -1348,14 +1337,25 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a6b3153b-6211-49e8-b9df-4ed7471cd786">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b68631fe-1afa-4047-a259-e724fa491ab9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C921D4C-07B4-4474-8EAC-015EFA022BA8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6C4C4AF-BD5A-4367-8747-177976D6CA92}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6C4C4AF-BD5A-4367-8747-177976D6CA92}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3476AF4A-3EAA-4603-B12E-865C6D04769F}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3476AF4A-3EAA-4603-B12E-865C6D04769F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C921D4C-07B4-4474-8EAC-015EFA022BA8}"/>
 </file>
</xml_diff>